<commit_message>
Fix error where variable OM costs did not sum to 1 for all plant types
</commit_message>
<xml_diff>
--- a/InputData/elec/SoESCaOMCbIC/Share of Electricity Sector Capital and OM Costs by ISIC Code.xlsx
+++ b/InputData/elec/SoESCaOMCbIC/Share of Electricity Sector Capital and OM Costs by ISIC Code.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\SoESCaOMCbIC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\SoESCaOMCbIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F8CB7E-4F9B-4533-81A3-FD34044A8A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36B3B44-873D-4041-9BDC-E6592614157F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="4" r:id="rId1"/>
@@ -2366,6 +2366,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2389,9 +2392,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2848,7 +2848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -3605,14 +3605,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="134" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="136"/>
+      <c r="A1" s="135" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="137"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -3934,14 +3934,14 @@
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="130" t="s">
+      <c r="A18" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="131"/>
-      <c r="C18" s="131"/>
-      <c r="D18" s="132"/>
-      <c r="E18" s="132"/>
-      <c r="F18" s="133"/>
+      <c r="B18" s="132"/>
+      <c r="C18" s="132"/>
+      <c r="D18" s="133"/>
+      <c r="E18" s="133"/>
+      <c r="F18" s="134"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="92" t="s">
@@ -4849,14 +4849,14 @@
     </row>
     <row r="74" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="75" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A75" s="134" t="s">
+      <c r="A75" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="B75" s="135"/>
-      <c r="C75" s="135"/>
-      <c r="D75" s="137"/>
-      <c r="E75" s="137"/>
-      <c r="F75" s="136"/>
+      <c r="B75" s="136"/>
+      <c r="C75" s="136"/>
+      <c r="D75" s="138"/>
+      <c r="E75" s="138"/>
+      <c r="F75" s="137"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
@@ -5458,14 +5458,14 @@
     </row>
     <row r="109" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="110" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A110" s="134" t="s">
+      <c r="A110" s="135" t="s">
         <v>41</v>
       </c>
-      <c r="B110" s="135"/>
-      <c r="C110" s="135"/>
-      <c r="D110" s="137"/>
-      <c r="E110" s="137"/>
-      <c r="F110" s="136"/>
+      <c r="B110" s="136"/>
+      <c r="C110" s="136"/>
+      <c r="D110" s="138"/>
+      <c r="E110" s="138"/>
+      <c r="F110" s="137"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
@@ -6059,14 +6059,14 @@
     </row>
     <row r="144" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="145" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A145" s="130" t="s">
+      <c r="A145" s="131" t="s">
         <v>52</v>
       </c>
-      <c r="B145" s="131"/>
-      <c r="C145" s="131"/>
-      <c r="D145" s="132"/>
-      <c r="E145" s="132"/>
-      <c r="F145" s="133"/>
+      <c r="B145" s="132"/>
+      <c r="C145" s="132"/>
+      <c r="D145" s="133"/>
+      <c r="E145" s="133"/>
+      <c r="F145" s="134"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
@@ -6385,14 +6385,14 @@
     </row>
     <row r="163" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="164" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A164" s="130" t="s">
+      <c r="A164" s="131" t="s">
         <v>71</v>
       </c>
-      <c r="B164" s="131"/>
-      <c r="C164" s="131"/>
-      <c r="D164" s="132"/>
-      <c r="E164" s="132"/>
-      <c r="F164" s="133"/>
+      <c r="B164" s="132"/>
+      <c r="C164" s="132"/>
+      <c r="D164" s="133"/>
+      <c r="E164" s="133"/>
+      <c r="F164" s="134"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
@@ -7371,14 +7371,14 @@
     </row>
     <row r="218" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="219" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A219" s="130" t="s">
+      <c r="A219" s="131" t="s">
         <v>226</v>
       </c>
-      <c r="B219" s="131"/>
-      <c r="C219" s="131"/>
-      <c r="D219" s="132"/>
-      <c r="E219" s="132"/>
-      <c r="F219" s="133"/>
+      <c r="B219" s="132"/>
+      <c r="C219" s="132"/>
+      <c r="D219" s="133"/>
+      <c r="E219" s="133"/>
+      <c r="F219" s="134"/>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
@@ -7654,14 +7654,14 @@
     </row>
     <row r="234" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="235" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A235" s="130" t="s">
+      <c r="A235" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="B235" s="131"/>
-      <c r="C235" s="131"/>
-      <c r="D235" s="132"/>
-      <c r="E235" s="132"/>
-      <c r="F235" s="133"/>
+      <c r="B235" s="132"/>
+      <c r="C235" s="132"/>
+      <c r="D235" s="133"/>
+      <c r="E235" s="133"/>
+      <c r="F235" s="134"/>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
@@ -8618,14 +8618,14 @@
       <c r="F288" s="10"/>
     </row>
     <row r="289" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A289" s="130" t="s">
+      <c r="A289" s="131" t="s">
         <v>337</v>
       </c>
-      <c r="B289" s="131"/>
-      <c r="C289" s="131"/>
-      <c r="D289" s="132"/>
-      <c r="E289" s="132"/>
-      <c r="F289" s="133"/>
+      <c r="B289" s="132"/>
+      <c r="C289" s="132"/>
+      <c r="D289" s="133"/>
+      <c r="E289" s="133"/>
+      <c r="F289" s="134"/>
     </row>
     <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="92" t="s">
@@ -9101,14 +9101,14 @@
       <c r="D314" s="101"/>
     </row>
     <row r="315" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A315" s="130" t="s">
+      <c r="A315" s="131" t="s">
         <v>365</v>
       </c>
-      <c r="B315" s="131"/>
-      <c r="C315" s="131"/>
-      <c r="D315" s="132"/>
-      <c r="E315" s="132"/>
-      <c r="F315" s="133"/>
+      <c r="B315" s="132"/>
+      <c r="C315" s="132"/>
+      <c r="D315" s="133"/>
+      <c r="E315" s="133"/>
+      <c r="F315" s="134"/>
     </row>
     <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" s="92" t="s">
@@ -19692,7 +19692,7 @@
       </c>
     </row>
     <row r="24" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A24" s="138" t="s">
+      <c r="A24" s="130" t="s">
         <v>511</v>
       </c>
       <c r="B24" s="77">
@@ -19865,7 +19865,7 @@
       </c>
     </row>
     <row r="25" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A25" s="138" t="s">
+      <c r="A25" s="130" t="s">
         <v>512</v>
       </c>
       <c r="B25" s="77">
@@ -24017,7 +24017,7 @@
       </c>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A24" s="138" t="s">
+      <c r="A24" s="130" t="s">
         <v>511</v>
       </c>
       <c r="B24" s="77">
@@ -24190,7 +24190,7 @@
       </c>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A25" s="138" t="s">
+      <c r="A25" s="130" t="s">
         <v>512</v>
       </c>
       <c r="B25" s="77">
@@ -24374,8 +24374,8 @@
   </sheetPr>
   <dimension ref="A1:AQ25"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:AQ25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:AQ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26668,7 +26668,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="89">
         <v>0</v>
@@ -26695,7 +26695,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15" s="89">
         <v>0</v>
@@ -28173,7 +28173,7 @@
       </c>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A24" s="138" t="s">
+      <c r="A24" s="130" t="s">
         <v>511</v>
       </c>
       <c r="B24" s="77">
@@ -28346,7 +28346,7 @@
       </c>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A25" s="138" t="s">
+      <c r="A25" s="130" t="s">
         <v>512</v>
       </c>
       <c r="B25" s="77">

</xml_diff>